<commit_message>
Añadinedo ASINs al fichero de descarga
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,40 +436,45 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>asins</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Imagen</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Título producto</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Precio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Precio caro</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Nún reviews</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Estrellas</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Descripcion</t>
         </is>
@@ -479,7 +484,11 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>B06WVXN3HQ</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -487,6 +496,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -494,34 +504,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://images-na.ssl-images-amazon.com/images/I/41SGHWok28L._AC_.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>B071LG3DDN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://images-na.ssl-images-amazon.com/images/I/41QeREFPHIL._AC_.jpg</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>FlowerW Cochecito de Bebé 78 x 60 x 107 CM, Carrito Bebé Silla de Paseo 78 x 60 x 107 CM, con Carro Multiuso, Silla de Paseo Ligera, Carro bebe, Carritos para Muñecas Plegado</t>
+          <t>Kk KinderKraft</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">118,99 </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>Kinderkraft Trona Bebé 2 en 1 FINI, Silla Infantil, Ajustable, Segura, Gris</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">89,00 </t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>131 valoraciones</t>
+          <t xml:space="preserve"> 99,00 </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>4,2 de 5 estrellas</t>
+          <t>2.807</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>【COCHECITO PARA BEBÉ PREMIUM】- Compatible: 0-36 meses bebé; capacidad de carga: 0-15 kg. Este cochecito de bebé presenta un asiento reversible que puede hacer que el bebé mire a la madre o la calle.</t>
+          <t>4,6</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>La bandeja ajustable en 3 niveles fácil Ita el envío al niño en la trona</t>
         </is>
       </c>
     </row>
@@ -529,7 +552,11 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B072LNHXLQ</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -537,12 +564,17 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B0785GR43J</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
@@ -550,6 +582,57 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B07GDVLMT5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://images-na.ssl-images-amazon.com/images/I/31KInCKXJlL._AC_.jpg</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Kinderkraft</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Kinderkraft Trona Bebé Ajustable Yummy, Segura, Bandeja, Hasta 3 los Años, Rosa</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">78,89 </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 84,90 </t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4,7</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>MULTIFUNCIONAL: YUMMY es una trona para bebé apta para los niños que pueden estar sentados solos (desde aprox. los 6 meses de vida) hasta que pesen un máximo de 15 kg (aprox. 3 años). Gracias a la opción de plegado a un tamaño compacto es muy fácil guardarla. También la podrás llevar contigo a las vacaciones</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>